<commit_message>
Updates to Academic Dishonesty
</commit_message>
<xml_diff>
--- a/Acedemic Dishonesty - GitHub/GitTest.xlsx
+++ b/Acedemic Dishonesty - GitHub/GitTest.xlsx
@@ -2,22 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickpichardo/Documents/GitHub/Research-Papers/Acedemic Dishonesty - GitHub/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickpichardo/Desktop/Spring 24/UGCA Spring/Research UGCA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE1D09C-9C38-B94F-9CE2-2972161BC99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42B7EC1-F4FF-E247-82EC-83D2B456570A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7160" yWindow="500" windowWidth="21640" windowHeight="16540" xr2:uid="{03CCA54B-6A87-BA4F-87B2-0800CDDB09CB}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16540" xr2:uid="{03CCA54B-6A87-BA4F-87B2-0800CDDB09CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1163,6 +1163,91 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1182,9 +1267,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.3108168562933017E-2"/>
-          <c:y val="3.6243335471309618E-2"/>
-          <c:w val="0.75059803772939104"/>
-          <c:h val="0.83761414413656476"/>
+          <c:y val="7.8884750422794359E-2"/>
+          <c:w val="0.85981624250098965"/>
+          <c:h val="0.79497280245037116"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -2059,15 +2144,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>306307</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>91012</xdr:rowOff>
+      <xdr:colOff>601352</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>161507</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>889000</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>200401</xdr:rowOff>
+      <xdr:colOff>1067537</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>67696</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2167,15 +2252,7 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="1"/>
     </cacheField>
     <cacheField name="Frequency per Search" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="7" count="7">
-        <n v="2"/>
-        <n v="0"/>
-        <n v="4"/>
-        <n v="6"/>
-        <n v="7"/>
-        <n v="5"/>
-        <n v="1"/>
-      </sharedItems>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="7"/>
     </cacheField>
     <cacheField name="Repo Links" numFmtId="0">
       <sharedItems/>
@@ -2203,7 +2280,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
-    <x v="0"/>
+    <n v="2"/>
     <s v="https://github.com/joshc-garcia/CS313E-Assignments"/>
   </r>
   <r>
@@ -2218,7 +2295,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
-    <x v="1"/>
+    <n v="0"/>
     <s v="https://github.com/lancefeig/cs313e_finalproject"/>
   </r>
   <r>
@@ -2233,7 +2310,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
-    <x v="1"/>
+    <n v="0"/>
     <s v="https://github.com/pranavkpradeep/CS313E"/>
   </r>
   <r>
@@ -2248,7 +2325,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
-    <x v="1"/>
+    <n v="0"/>
     <s v="https://github.com/uploadtigris/CS313E_Readings"/>
   </r>
   <r>
@@ -2263,7 +2340,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
-    <x v="2"/>
+    <n v="4"/>
     <s v="https://github.com/Minouneshan/CS313E-UTAustin"/>
   </r>
   <r>
@@ -2278,7 +2355,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="1"/>
-    <x v="2"/>
+    <n v="4"/>
     <s v="https://github.com/halil-hamscho/CS313E"/>
   </r>
   <r>
@@ -2293,7 +2370,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="1"/>
-    <x v="2"/>
+    <n v="4"/>
     <s v="https://github.com/sashi8a/CS313E"/>
   </r>
   <r>
@@ -2308,7 +2385,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
-    <x v="2"/>
+    <n v="4"/>
     <s v="https://github.com/austinjp17/cs313E"/>
   </r>
   <r>
@@ -2323,7 +2400,7 @@
     <n v="0"/>
     <n v="1"/>
     <n v="1"/>
-    <x v="3"/>
+    <n v="6"/>
     <s v="https://github.com/raqmejtru/CS313E_Elements_of_Software_Design"/>
   </r>
   <r>
@@ -2338,7 +2415,7 @@
     <n v="0"/>
     <n v="1"/>
     <n v="1"/>
-    <x v="4"/>
+    <n v="7"/>
     <s v="https://github.com/tylersmed/cs313"/>
   </r>
   <r>
@@ -2353,7 +2430,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="1"/>
-    <x v="5"/>
+    <n v="5"/>
     <s v="https://github.com/Julian-Wearden-UT/Fall2021_CS313E_Projects"/>
   </r>
   <r>
@@ -2368,7 +2445,7 @@
     <n v="0"/>
     <n v="1"/>
     <n v="1"/>
-    <x v="4"/>
+    <n v="7"/>
     <s v="https://github.com/makutexas/Fall22-CS313E-Assignments"/>
   </r>
   <r>
@@ -2383,7 +2460,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
-    <x v="6"/>
+    <n v="1"/>
     <s v="https://github.com/kellyhyun/cs313e"/>
   </r>
   <r>
@@ -2398,7 +2475,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
-    <x v="6"/>
+    <n v="1"/>
     <s v="https://github.com/ck27924/CS313E-Work"/>
   </r>
   <r>
@@ -2413,7 +2490,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="1"/>
-    <x v="3"/>
+    <n v="6"/>
     <s v="https://github.com/enya126/Python-2---software-design"/>
   </r>
   <r>
@@ -2428,7 +2505,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="1"/>
-    <x v="3"/>
+    <n v="6"/>
     <s v="https://github.com/morgan-handojo/CS-Work-Fall-2023"/>
   </r>
   <r>
@@ -2443,7 +2520,7 @@
     <n v="0"/>
     <n v="1"/>
     <n v="1"/>
-    <x v="3"/>
+    <n v="6"/>
     <s v="https://github.com/raqmejtru/CS313E_Elements_of_Software_Design"/>
   </r>
   <r>
@@ -2458,7 +2535,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="1"/>
-    <x v="5"/>
+    <n v="5"/>
     <s v="https://github.com/AmberEtana/Elements-of-Software-Design"/>
   </r>
   <r>
@@ -2473,7 +2550,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
-    <x v="6"/>
+    <n v="1"/>
     <s v="https://github.com/carlaigonzalez/CS313E"/>
   </r>
   <r>
@@ -2488,7 +2565,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
-    <x v="1"/>
+    <n v="0"/>
     <s v="https://github.com/ankitasumeet17/CS313E-Elements-of-Software-Design"/>
   </r>
   <r>
@@ -2503,7 +2580,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
-    <x v="1"/>
+    <n v="0"/>
     <s v="https://github.com/FelixLuciano/Elements-of-Software-Design"/>
   </r>
   <r>
@@ -2518,7 +2595,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
-    <x v="1"/>
+    <n v="0"/>
     <s v="https://github.com/jpkrajewski/software-design-patterns"/>
   </r>
   <r>
@@ -2533,7 +2610,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
-    <x v="1"/>
+    <n v="0"/>
     <s v="https://github.com/maxedout2/CS-313-Elements-of-Software-Design"/>
   </r>
   <r>
@@ -2548,7 +2625,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="1"/>
-    <x v="3"/>
+    <n v="6"/>
     <s v="https://github.com/enya126/Python-2---software-design"/>
   </r>
   <r>
@@ -2563,7 +2640,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
-    <x v="6"/>
+    <n v="1"/>
     <s v="https://github.com/alicianireland/CS313E"/>
   </r>
   <r>
@@ -2578,7 +2655,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="1"/>
-    <x v="5"/>
+    <n v="5"/>
     <s v="https://github.com/jenny-fotso/Elements-of-Software-Design"/>
   </r>
   <r>
@@ -2593,7 +2670,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
-    <x v="6"/>
+    <n v="1"/>
     <s v="https://github.com/ashlilii/CS313E"/>
   </r>
   <r>
@@ -2608,7 +2685,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
-    <x v="1"/>
+    <n v="0"/>
     <s v="https://github.com/Hugo-cruz/design-patterns-python"/>
   </r>
   <r>
@@ -2623,7 +2700,7 @@
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
-    <x v="1"/>
+    <n v="0"/>
     <s v="https://github.com/pranj2000/Python-Programming-Projects"/>
   </r>
   <r>
@@ -2638,14 +2715,14 @@
     <n v="0"/>
     <n v="0"/>
     <n v="1"/>
-    <x v="3"/>
+    <n v="6"/>
     <s v="https://github.com/OCoderO/Elements-of-Software-Design---UT-Austin"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9BFA917-7D02-3041-A129-7EBB9380B1B5}" name="PivotTable2" cacheId="11" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C9BFA917-7D02-3041-A129-7EBB9380B1B5}" name="PivotTable2" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="C34:D43" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0">
@@ -2665,18 +2742,7 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="8">
-        <item x="1"/>
-        <item x="6"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="5"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
@@ -2725,7 +2791,7 @@
     <dataField name="Sum of 09 Image Bucket Fill" fld="9" baseField="0" baseItem="0"/>
     <dataField name="Sum of 10 Topological Sort" fld="10" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="9">
+  <chartFormats count="11">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -2803,6 +2869,24 @@
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="16" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="17" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -3157,8 +3241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C9F959-086B-3D41-BB93-140D9A02CCC4}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" zoomScale="75" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3166,7 +3250,7 @@
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
     <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.33203125" customWidth="1"/>
     <col min="7" max="7" width="23.33203125" bestFit="1" customWidth="1"/>
@@ -4035,6 +4119,9 @@
         <v>1</v>
       </c>
       <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">

</xml_diff>